<commit_message>
2022 mens WC final scores
claude assisted: https://claude.ai/share/e1fc61e5-3e86-45e7-8b69-32ee1c6f221c
</commit_message>
<xml_diff>
--- a/src/stp/database/2022-mens-world-cup.xlsx
+++ b/src/stp/database/2022-mens-world-cup.xlsx
@@ -1,28 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCAD34C-66C2-A549-BE43-096913287F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2370D2A-D694-F848-B362-EC0DB4830186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tournament" sheetId="8" r:id="rId1"/>
-    <sheet name="Matches" sheetId="1" r:id="rId2"/>
+    <sheet name="Tournament" sheetId="1" r:id="rId1"/>
+    <sheet name="Matches" sheetId="2" r:id="rId2"/>
     <sheet name="Seeds" sheetId="3" r:id="rId3"/>
-    <sheet name="Colors" sheetId="9" r:id="rId4"/>
+    <sheet name="Colors" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -39,7 +36,247 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="203">
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>World Cup 2022 in Qatar</t>
+  </si>
+  <si>
+    <t>Copa del Mundo 2022 en Qatar</t>
+  </si>
+  <si>
+    <t>Mondiali 2022 in Qatar</t>
+  </si>
+  <si>
+    <t>Coupe du monde 2022 au Qatar</t>
+  </si>
+  <si>
+    <t>WM 2022 in Katar</t>
+  </si>
+  <si>
+    <t>WK voetbal 2022 - Qatar</t>
+  </si>
+  <si>
+    <t>2022カタールW杯</t>
+  </si>
+  <si>
+    <t>جام جهانی 2022 در قطر</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>W.C. 2022 Schedule &amp; Score Card</t>
+  </si>
+  <si>
+    <t>Card de calificación y puntaje 2022</t>
+  </si>
+  <si>
+    <t>2022 Scheda di programma e punteggio</t>
+  </si>
+  <si>
+    <t>2022 Calendrier et carte de score</t>
+  </si>
+  <si>
+    <t>2022 Zeitplan- und Score -Karte</t>
+  </si>
+  <si>
+    <t>2022 Schema &amp; scorekaart</t>
+  </si>
+  <si>
+    <t>2022W杯 日程・スコア</t>
+  </si>
+  <si>
+    <t>جام جهانی 2022 برنامه و کارت امتیاز</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Katar</t>
+  </si>
+  <si>
+    <t>カタール</t>
+  </si>
+  <si>
+    <t>قطر</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>Asia/Qatar</t>
+  </si>
+  <si>
+    <t>venue.1</t>
+  </si>
+  <si>
+    <t>Al Bayt</t>
+  </si>
+  <si>
+    <t>الحاق</t>
+  </si>
+  <si>
+    <t>venue.2</t>
+  </si>
+  <si>
+    <t>Khalifa Internat.</t>
+  </si>
+  <si>
+    <t>ハリファインターナショナル</t>
+  </si>
+  <si>
+    <t>خلیفه بین المللی</t>
+  </si>
+  <si>
+    <t>venue.3</t>
+  </si>
+  <si>
+    <t>Al Thumama</t>
+  </si>
+  <si>
+    <t>アル・トゥママ</t>
+  </si>
+  <si>
+    <t>ایل تومااما</t>
+  </si>
+  <si>
+    <t>venue.4</t>
+  </si>
+  <si>
+    <t>Ahmad Bin Ali</t>
+  </si>
+  <si>
+    <t>アフマド・ビン・アリ</t>
+  </si>
+  <si>
+    <t>احمد بن علی</t>
+  </si>
+  <si>
+    <t>venue.5</t>
+  </si>
+  <si>
+    <t>Lusail</t>
+  </si>
+  <si>
+    <t>ルセイル</t>
+  </si>
+  <si>
+    <t>لوسیل</t>
+  </si>
+  <si>
+    <t>venue.6</t>
+  </si>
+  <si>
+    <t>Stadium 974</t>
+  </si>
+  <si>
+    <t>Estadio 974</t>
+  </si>
+  <si>
+    <t>Stadio 974</t>
+  </si>
+  <si>
+    <t>Stade 974</t>
+  </si>
+  <si>
+    <t>Stadion 974</t>
+  </si>
+  <si>
+    <t>スタジアム974</t>
+  </si>
+  <si>
+    <t>استادیوم 974</t>
+  </si>
+  <si>
+    <t>venue.7</t>
+  </si>
+  <si>
+    <t>Education City</t>
+  </si>
+  <si>
+    <t>教育都市</t>
+  </si>
+  <si>
+    <t>شهر آموزش</t>
+  </si>
+  <si>
+    <t>venue.8</t>
+  </si>
+  <si>
+    <t>Al Janoub</t>
+  </si>
+  <si>
+    <t>アル・ジャノウブ</t>
+  </si>
+  <si>
+    <t>ال ژانوب</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>home-seed</t>
+  </si>
+  <si>
+    <t>away-seed</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>home-team</t>
+  </si>
+  <si>
+    <t>away-team</t>
+  </si>
+  <si>
+    <t>home-score</t>
+  </si>
+  <si>
+    <t>away-score</t>
+  </si>
+  <si>
+    <t>home-tiebreaker</t>
+  </si>
+  <si>
+    <t>away-tiebreaker</t>
+  </si>
   <si>
     <t>A1</t>
   </si>
@@ -47,96 +284,192 @@
     <t>A2</t>
   </si>
   <si>
+    <t>QAT</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
     <t>A3</t>
   </si>
   <si>
     <t>A4</t>
   </si>
   <si>
+    <t>SEN</t>
+  </si>
+  <si>
+    <t>NED</t>
+  </si>
+  <si>
     <t>B1</t>
   </si>
   <si>
     <t>B2</t>
   </si>
   <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>IRN</t>
+  </si>
+  <si>
     <t>B3</t>
   </si>
   <si>
     <t>B4</t>
   </si>
   <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>WAL</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
     <t>D3</t>
   </si>
   <si>
     <t>D4</t>
   </si>
   <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>TUN</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
     <t>C4</t>
   </si>
   <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>KSA</t>
+  </si>
+  <si>
     <t>F1</t>
   </si>
   <si>
     <t>F2</t>
   </si>
   <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
     <t>E2</t>
   </si>
   <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
     <t>E3</t>
   </si>
   <si>
     <t>E4</t>
   </si>
   <si>
+    <t>GER</t>
+  </si>
+  <si>
+    <t>JPN</t>
+  </si>
+  <si>
     <t>F3</t>
   </si>
   <si>
     <t>F4</t>
   </si>
   <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>CRO</t>
+  </si>
+  <si>
     <t>G3</t>
   </si>
   <si>
     <t>G4</t>
   </si>
   <si>
+    <t>SUI</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
     <t>H3</t>
   </si>
   <si>
     <t>H4</t>
   </si>
   <si>
+    <t>URU</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
     <t>H1</t>
   </si>
   <si>
     <t>H2</t>
   </si>
   <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
     <t>G1</t>
   </si>
   <si>
     <t>G2</t>
   </si>
   <si>
+    <t>BRA</t>
+  </si>
+  <si>
+    <t>SRB</t>
+  </si>
+  <si>
     <t>1A</t>
   </si>
   <si>
@@ -221,433 +554,97 @@
     <t>W60</t>
   </si>
   <si>
+    <t>L61</t>
+  </si>
+  <si>
+    <t>L62</t>
+  </si>
+  <si>
     <t>W61</t>
   </si>
   <si>
     <t>W62</t>
   </si>
   <si>
-    <t>match</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>Al Bayt</t>
-  </si>
-  <si>
-    <t>Khalifa Internat.</t>
-  </si>
-  <si>
-    <t>Al Thumama</t>
-  </si>
-  <si>
-    <t>Ahmad Bin Ali</t>
-  </si>
-  <si>
-    <t>Lusail</t>
-  </si>
-  <si>
-    <t>Stadium 974</t>
-  </si>
-  <si>
-    <t>Education City</t>
-  </si>
-  <si>
-    <t>Al Janoub</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>seed</t>
   </si>
   <si>
-    <t>BRA</t>
-  </si>
-  <si>
-    <t>BEL</t>
-  </si>
-  <si>
-    <t>FRA</t>
-  </si>
-  <si>
-    <t>ARG</t>
-  </si>
-  <si>
-    <t>ENG</t>
-  </si>
-  <si>
-    <t>POR</t>
-  </si>
-  <si>
-    <t>MEX</t>
-  </si>
-  <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>GER</t>
-  </si>
-  <si>
-    <t>URU</t>
-  </si>
-  <si>
-    <t>CRO</t>
-  </si>
-  <si>
-    <t>WAL</t>
-  </si>
-  <si>
-    <t>SEN</t>
-  </si>
-  <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>AUS</t>
-  </si>
-  <si>
-    <t>TUN</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>ESP</t>
-  </si>
-  <si>
-    <t>SUI</t>
-  </si>
-  <si>
-    <t>JPN</t>
-  </si>
-  <si>
-    <t>KOR</t>
-  </si>
-  <si>
-    <t>CRC</t>
-  </si>
-  <si>
-    <t>SRB</t>
-  </si>
-  <si>
-    <t>MAR</t>
-  </si>
-  <si>
-    <t>IRN</t>
-  </si>
-  <si>
-    <t>ECU</t>
-  </si>
-  <si>
-    <t>KSA</t>
-  </si>
-  <si>
-    <t>QAT</t>
-  </si>
-  <si>
-    <t>GHA</t>
-  </si>
-  <si>
-    <t>NED</t>
-  </si>
-  <si>
-    <t>CMR</t>
-  </si>
-  <si>
-    <t>L61</t>
-  </si>
-  <si>
-    <t>L62</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>Katar</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>nl</t>
-  </si>
-  <si>
-    <t>venue.1</t>
-  </si>
-  <si>
-    <t>venue.2</t>
-  </si>
-  <si>
-    <t>venue.3</t>
-  </si>
-  <si>
-    <t>venue.4</t>
-  </si>
-  <si>
-    <t>venue.5</t>
-  </si>
-  <si>
-    <t>venue.6</t>
-  </si>
-  <si>
-    <t>venue.7</t>
-  </si>
-  <si>
-    <t>venue.8</t>
-  </si>
-  <si>
-    <t>Estadio 974</t>
-  </si>
-  <si>
-    <t>Stadio 974</t>
-  </si>
-  <si>
-    <t>Stade 974</t>
-  </si>
-  <si>
-    <t>Stadion 974</t>
-  </si>
-  <si>
-    <t>World Cup 2022 in Qatar</t>
-  </si>
-  <si>
-    <t>Copa del Mundo 2022 en Qatar</t>
-  </si>
-  <si>
-    <t>Mondiali 2022 in Qatar</t>
-  </si>
-  <si>
-    <t>Coupe du monde 2022 au Qatar</t>
-  </si>
-  <si>
-    <t>WM 2022 in Katar</t>
-  </si>
-  <si>
-    <t>WK voetbal 2022 - Qatar</t>
-  </si>
-  <si>
-    <t>Card de calificación y puntaje 2022</t>
-  </si>
-  <si>
-    <t>2022 Scheda di programma e punteggio</t>
-  </si>
-  <si>
-    <t>2022 Calendrier et carte de score</t>
-  </si>
-  <si>
-    <t>2022 Zeitplan- und Score -Karte</t>
-  </si>
-  <si>
-    <t>2022 Schema &amp; scorekaart</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>جام جهانی 2022 در قطر</t>
-  </si>
-  <si>
-    <t>قطر</t>
-  </si>
-  <si>
-    <t>カタール</t>
-  </si>
-  <si>
-    <t>الحاق</t>
-  </si>
-  <si>
-    <t>ハリファインターナショナル</t>
-  </si>
-  <si>
-    <t>خلیفه بین المللی</t>
-  </si>
-  <si>
-    <t>アル・トゥママ</t>
-  </si>
-  <si>
-    <t>ایل تومااما</t>
-  </si>
-  <si>
-    <t>アフマド・ビン・アリ</t>
-  </si>
-  <si>
-    <t>احمد بن علی</t>
-  </si>
-  <si>
-    <t>ルセイル</t>
-  </si>
-  <si>
-    <t>لوسیل</t>
-  </si>
-  <si>
-    <t>スタジアム974</t>
-  </si>
-  <si>
-    <t>استادیوم 974</t>
-  </si>
-  <si>
-    <t>教育都市</t>
-  </si>
-  <si>
-    <t>شهر آموزش</t>
-  </si>
-  <si>
-    <t>アル・ジャノウブ</t>
-  </si>
-  <si>
-    <t>ال ژانوب</t>
-  </si>
-  <si>
-    <t>home-score</t>
-  </si>
-  <si>
-    <t>away-score</t>
-  </si>
-  <si>
-    <t>away-tiebreaker</t>
-  </si>
-  <si>
-    <t>home-tiebreaker</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>W.C. 2022 Schedule &amp; Score Card</t>
-  </si>
-  <si>
     <t>team</t>
   </si>
   <si>
-    <t>جام جهانی 2022 برنامه و کارت امتیاز</t>
-  </si>
-  <si>
-    <t>home-seed</t>
-  </si>
-  <si>
-    <t>away-seed</t>
-  </si>
-  <si>
-    <t>home-team</t>
-  </si>
-  <si>
-    <t>away-team</t>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>#94d9f5</t>
+  </si>
+  <si>
+    <t>pale cyan</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>#fee289</t>
+  </si>
+  <si>
+    <t>pale yellow</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>#f79d8f</t>
+  </si>
+  <si>
+    <t>pale red</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>#c4e1b5</t>
+  </si>
+  <si>
+    <t>pale green</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>#b0d0ee</t>
+  </si>
+  <si>
+    <t>pale blue</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>#c0e4df</t>
+  </si>
+  <si>
+    <t>pale teal</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>#fab077</t>
+  </si>
+  <si>
+    <t>pale orange</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>#eecbef</t>
   </si>
   <si>
     <t>pale purple</t>
-  </si>
-  <si>
-    <t>#eecbef</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>pale orange</t>
-  </si>
-  <si>
-    <t>#fab077</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>pale teal</t>
-  </si>
-  <si>
-    <t>#c0e4df</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>pale blue</t>
-  </si>
-  <si>
-    <t>#b0d0ee</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>pale green</t>
-  </si>
-  <si>
-    <t>#c4e1b5</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>pale red</t>
-  </si>
-  <si>
-    <t>#f79d8f</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>pale yellow</t>
-  </si>
-  <si>
-    <t>#fee289</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>pale cyan</t>
-  </si>
-  <si>
-    <t>#94d9f5</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>timezone</t>
-  </si>
-  <si>
-    <t>Asia/Qatar</t>
-  </si>
-  <si>
-    <t>2022W杯 日程・スコア</t>
-  </si>
-  <si>
-    <t>2022カタールW杯</t>
   </si>
 </sst>
 </file>
@@ -657,16 +654,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -701,7 +692,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,68 +727,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I13" totalsRowShown="0">
-  <autoFilter ref="A1:I13" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tournament" displayName="tournament" ref="A1:I13" totalsRowShown="0">
+  <autoFilter ref="A1:I13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A8CDEDD3-FA49-4AD4-8D9F-D3DFCABC2052}" name="key"/>
-    <tableColumn id="2" xr3:uid="{88778009-1F1A-4B0F-BCE2-A71F4DD7CF67}" name="en"/>
-    <tableColumn id="3" xr3:uid="{B0854098-6051-4EC6-B153-6F15A5D8EDE3}" name="es"/>
-    <tableColumn id="4" xr3:uid="{451E0539-ECF2-4BD5-A71E-337F41B0AED7}" name="it"/>
-    <tableColumn id="5" xr3:uid="{B50399C0-B1D0-4B7B-9997-0B86C7572F77}" name="fr"/>
-    <tableColumn id="6" xr3:uid="{B0F7BA24-53BA-4D61-BC1C-8F39E4CFC9AD}" name="de"/>
-    <tableColumn id="7" xr3:uid="{F2DB2A1A-9388-4CD2-9231-4B516407345F}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{E069B466-BE62-49FE-858B-990B30F1EE20}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{29A41F5D-C82C-4A8F-B732-857BFD0D7766}" name="fa"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="es"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="it"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="fr"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="de"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="nl"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ja"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="fa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:K65" totalsRowShown="0">
-  <autoFilter ref="A1:K65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="matches" displayName="matches" ref="A1:K65" totalsRowShown="0">
+  <autoFilter ref="A1:K65" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
-    <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
-    <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
-    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="match"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="home-seed"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="away-seed"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="time"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="venue" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="home-team"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="away-team"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="home-score" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="away-score" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="home-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="away-tiebreaker" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}" name="seeds" displayName="seeds" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="seeds" displayName="seeds" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C0AEBB99-51D0-46B6-ACD7-C4F2DC461A4C}" name="seed"/>
-    <tableColumn id="3" xr3:uid="{DD8C8688-8EED-4B48-9C61-D766CD3EFBBB}" name="team"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="seed"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="team"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DF7CDC91-A33A-4A72-9C3F-156105A85ED8}" name="groups" displayName="groups" ref="A1:J9" totalsRowShown="0">
-  <autoFilter ref="A1:J9" xr:uid="{4B86982E-77B7-4963-838F-4D594C24841B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="groups" displayName="groups" ref="A1:J9" totalsRowShown="0">
+  <autoFilter ref="A1:J9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D0E0E528-2BCB-4298-80EB-394686B036E7}" name="key"/>
-    <tableColumn id="2" xr3:uid="{3AD006A1-BF1D-4EE6-A45C-16FF2881DC52}" name="en"/>
-    <tableColumn id="3" xr3:uid="{26579E3F-BC15-4480-AD0D-BD2B2AE4B0AF}" name="es"/>
-    <tableColumn id="4" xr3:uid="{8BAB4BAD-FFFD-44D1-A4E3-0774FD0BAC15}" name="it"/>
-    <tableColumn id="5" xr3:uid="{3222D3A2-26F6-4B50-B423-C40487FE1EC4}" name="fr"/>
-    <tableColumn id="6" xr3:uid="{616BCBD8-3581-4F2F-9B1C-31ACE35035FE}" name="de"/>
-    <tableColumn id="7" xr3:uid="{9A002B4D-A4A3-4BEA-81E5-703F21AC9DC0}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{B552B0B0-7C97-4F30-A9B3-F5664D12EED8}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{1CE81ADD-EB4A-43B1-B848-8A2AFC0016C4}" name="fa"/>
-    <tableColumn id="10" xr3:uid="{7FD91AD2-7E21-4D2A-901D-ED242D54C2F0}" name="notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="key"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="en"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="es"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="it"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="fr"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="de"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="nl"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="ja"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="fa"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1099,10 +1090,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1124,376 +1115,375 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>202</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>201</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,37 +1497,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>172</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s">
-        <v>162</v>
+        <v>77</v>
       </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1545,724 +1535,1064 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D2" s="1">
-        <v>44885.666666666664</v>
+        <v>44885.666666666657</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="F2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>QAT</v>
+      </c>
+      <c r="G2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1">
-        <v>44886.666666666664</v>
+        <v>44886.666666666657</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="F3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SEN</v>
+      </c>
+      <c r="G3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1">
-        <v>44886.541666666664</v>
+        <v>44886.541666666657</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="F4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
+      <c r="G4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>IRN</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1">
-        <v>44886.791666666664</v>
+        <v>44886.791666666657</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="F5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="G5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>WAL</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="D6" s="1">
-        <v>44887.791666666664</v>
+        <v>44887.791666666657</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="F6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
+      <c r="G6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1">
-        <v>44887.541666666664</v>
+        <v>44887.541666666657</v>
       </c>
       <c r="E7">
         <v>7</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="F7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
+      <c r="G7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>TUN</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1">
-        <v>44887.666666666664</v>
+        <v>44887.666666666657</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="F8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
+      <c r="G8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>POL</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1">
-        <v>44887.416666666664</v>
+        <v>44887.416666666657</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="F9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>KSA</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1">
-        <v>44888.791666666664</v>
+        <v>44888.791666666657</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="F10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BEL</v>
+      </c>
+      <c r="G10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1">
-        <v>44888.666666666664</v>
+        <v>44888.666666666657</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="F11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
+      <c r="G11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1">
-        <v>44888.541666666664</v>
+        <v>44888.541666666657</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="F12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
+      <c r="G12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="D13" s="1">
-        <v>44888.416666666664</v>
+        <v>44888.416666666657</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="F13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
+      <c r="G13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRO</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="D14" s="1">
-        <v>44889.416666666664</v>
+        <v>44889.416666666657</v>
       </c>
       <c r="E14">
         <v>8</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="F14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
+      <c r="G14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CMR</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="D15" s="1">
-        <v>44889.541666666664</v>
+        <v>44889.541666666657</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="F15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
+      <c r="G15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="D16" s="1">
-        <v>44889.666666666664</v>
+        <v>44889.666666666657</v>
       </c>
       <c r="E16">
         <v>6</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
+      <c r="G16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>GHA</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D17" s="1">
-        <v>44889.791666666664</v>
+        <v>44889.791666666657</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="G17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SRB</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1">
-        <v>44890.416666666664</v>
+        <v>44890.416666666657</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>WAL</v>
+      </c>
+      <c r="G18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>IRN</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1">
-        <v>44890.541666666664</v>
+        <v>44890.541666666657</v>
       </c>
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>QAT</v>
+      </c>
+      <c r="G19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SEN</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1">
-        <v>44890.666666666664</v>
+        <v>44890.666666666657</v>
       </c>
       <c r="E20">
         <v>2</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
+      <c r="G20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1">
-        <v>44890.791666666664</v>
+        <v>44890.791666666657</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
+      <c r="G21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1">
-        <v>44891.416666666664</v>
+        <v>44891.416666666657</v>
       </c>
       <c r="E22">
         <v>8</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>TUN</v>
+      </c>
+      <c r="G22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="D23" s="1">
-        <v>44891.541666666664</v>
+        <v>44891.541666666657</v>
       </c>
       <c r="E23">
         <v>7</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POL</v>
+      </c>
+      <c r="G23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>KSA</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1">
-        <v>44891.666666666664</v>
+        <v>44891.666666666657</v>
       </c>
       <c r="E24">
         <v>6</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
+      <c r="G24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="D25" s="1">
-        <v>44891.791666666664</v>
+        <v>44891.791666666657</v>
       </c>
       <c r="E25">
         <v>5</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="D26" s="1">
-        <v>44892.416666666664</v>
+        <v>44892.416666666657</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F26" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
+      <c r="G26" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="D27" s="1">
-        <v>44892.541666666664</v>
+        <v>44892.541666666657</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F27" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BEL</v>
+      </c>
+      <c r="G27" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D28" s="1">
-        <v>44892.666666666664</v>
+        <v>44892.666666666657</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F28" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CRO</v>
+      </c>
+      <c r="G28" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="D29" s="1">
-        <v>44892.791666666664</v>
+        <v>44892.791666666657</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F29" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
+      <c r="G29" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D30" s="1">
-        <v>44893.416666666664</v>
+        <v>44893.416666666657</v>
       </c>
       <c r="E30">
         <v>8</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F30" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CMR</v>
+      </c>
+      <c r="G30" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SRB</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1">
-        <v>44893.541666666664</v>
+        <v>44893.541666666657</v>
       </c>
       <c r="E31">
         <v>7</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F31" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
+      <c r="G31" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>GHA</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="D32" s="1">
-        <v>44893.666666666664</v>
+        <v>44893.666666666657</v>
       </c>
       <c r="E32">
         <v>6</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F32" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="G32" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="D33" s="1">
-        <v>44893.791666666664</v>
+        <v>44893.791666666657</v>
       </c>
       <c r="E33">
         <v>5</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F33" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
+      <c r="G33" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="D34" s="1">
-        <v>44894.791666666664</v>
+        <v>44894.791666666657</v>
       </c>
       <c r="E34">
         <v>4</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F34" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>WAL</v>
+      </c>
+      <c r="G34" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D35" s="1">
-        <v>44894.791666666664</v>
+        <v>44894.791666666657</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F35" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>IRN</v>
+      </c>
+      <c r="G35" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1">
         <v>44894.625</v>
@@ -2270,20 +2600,30 @@
       <c r="E36">
         <v>2</v>
       </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F36" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
+      <c r="G36" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SEN</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D37" s="1">
         <v>44894.625</v>
@@ -2291,20 +2631,30 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F37" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
+      <c r="G37" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>QAT</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D38" s="1">
         <v>44895.625</v>
@@ -2312,20 +2662,30 @@
       <c r="E38">
         <v>8</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F38" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
+      <c r="G38" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1">
         <v>44895.625</v>
@@ -2333,62 +2693,92 @@
       <c r="E39">
         <v>7</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F39" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>TUN</v>
+      </c>
+      <c r="G39" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="D40" s="1">
-        <v>44895.791666666664</v>
+        <v>44895.791666666657</v>
       </c>
       <c r="E40">
         <v>6</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F40" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POL</v>
+      </c>
+      <c r="G40" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="D41" s="1">
-        <v>44895.791666666664</v>
+        <v>44895.791666666657</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F41" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>KSA</v>
+      </c>
+      <c r="G41" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="D42" s="1">
         <v>44896.625</v>
@@ -2396,20 +2786,30 @@
       <c r="E42">
         <v>4</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F42" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CRO</v>
+      </c>
+      <c r="G42" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BEL</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="D43" s="1">
         <v>44896.625</v>
@@ -2417,62 +2817,92 @@
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F43" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="G43" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1">
-        <v>44896.791666666664</v>
+        <v>44896.791666666657</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F44" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
+      <c r="G44" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1">
-        <v>44896.791666666664</v>
+        <v>44896.791666666657</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F45" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
+      <c r="G45" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="D46" s="1">
         <v>44897.625</v>
@@ -2480,20 +2910,30 @@
       <c r="E46">
         <v>8</v>
       </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F46" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>GHA</v>
+      </c>
+      <c r="G46" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="D47" s="1">
         <v>44897.625</v>
@@ -2501,62 +2941,92 @@
       <c r="E47">
         <v>7</v>
       </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F47" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
+      <c r="G47" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="D48" s="1">
-        <v>44897.791666666664</v>
+        <v>44897.791666666657</v>
       </c>
       <c r="E48">
         <v>6</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
+      <c r="F48" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SRB</v>
+      </c>
+      <c r="G48" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D49" s="1">
-        <v>44897.791666666664</v>
+        <v>44897.791666666657</v>
       </c>
       <c r="E49">
         <v>5</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
+      <c r="F49" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CMR</v>
+      </c>
+      <c r="G49" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>145</v>
       </c>
       <c r="D50" s="1">
         <v>44898.625</v>
@@ -2564,62 +3034,86 @@
       <c r="E50">
         <v>2</v>
       </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="F50" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>147</v>
       </c>
       <c r="D51" s="1">
-        <v>44898.791666666664</v>
+        <v>44898.791666666657</v>
       </c>
       <c r="E51">
         <v>4</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
+      <c r="F51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G51" t="s">
+        <v>99</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="D52" s="1">
-        <v>44899.791666666664</v>
+        <v>44899.791666666657</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="F52" t="s">
+        <v>98</v>
+      </c>
+      <c r="G52" t="s">
+        <v>107</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="D53" s="1">
         <v>44899.625</v>
@@ -2627,20 +3121,28 @@
       <c r="E53">
         <v>3</v>
       </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="F53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" t="s">
+        <v>86</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="D54" s="1">
         <v>44900.625</v>
@@ -2648,41 +3150,63 @@
       <c r="E54">
         <v>8</v>
       </c>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="F54" t="s">
+        <v>123</v>
+      </c>
+      <c r="G54" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="D55" s="1">
-        <v>44900.791666666664</v>
+        <v>44900.791666666657</v>
       </c>
       <c r="E55">
         <v>6</v>
       </c>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
+      <c r="F55" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" t="s">
+        <v>135</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="D56" s="1">
         <v>44901.625</v>
@@ -2690,62 +3214,98 @@
       <c r="E56">
         <v>7</v>
       </c>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
+      <c r="F56" t="s">
+        <v>126</v>
+      </c>
+      <c r="G56" t="s">
+        <v>118</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>3</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="D57" s="1">
-        <v>44901.791666666664</v>
+        <v>44901.791666666657</v>
       </c>
       <c r="E57">
         <v>5</v>
       </c>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
+      <c r="F57" t="s">
+        <v>138</v>
+      </c>
+      <c r="G57" t="s">
+        <v>130</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="D58" s="1">
-        <v>44904.791666666664</v>
+        <v>44904.791666666657</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="F58" t="s">
+        <v>127</v>
+      </c>
+      <c r="G58" t="s">
+        <v>142</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="D59" s="1">
         <v>44904.625</v>
@@ -2753,41 +3313,63 @@
       <c r="E59">
         <v>7</v>
       </c>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
+      <c r="F59" t="s">
+        <v>87</v>
+      </c>
+      <c r="G59" t="s">
+        <v>110</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>3</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>164</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
       <c r="D60" s="1">
-        <v>44905.791666666664</v>
+        <v>44905.791666666657</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
+      <c r="F60" t="s">
+        <v>126</v>
+      </c>
+      <c r="G60" t="s">
+        <v>138</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="D61" s="1">
         <v>44905.625</v>
@@ -2795,62 +3377,86 @@
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
+      <c r="F61" t="s">
+        <v>90</v>
+      </c>
+      <c r="G61" t="s">
+        <v>98</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
       <c r="D62" s="1">
-        <v>44908.791666666664</v>
+        <v>44908.791666666657</v>
       </c>
       <c r="E62">
         <v>5</v>
       </c>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
+      <c r="F62" t="s">
+        <v>110</v>
+      </c>
+      <c r="G62" t="s">
+        <v>127</v>
+      </c>
+      <c r="H62">
+        <v>3</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
       <c r="D63" s="1">
-        <v>44909.791666666664</v>
+        <v>44909.791666666657</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="F63" t="s">
+        <v>98</v>
+      </c>
+      <c r="G63" t="s">
+        <v>126</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="C64" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="D64" s="1">
         <v>44912.625</v>
@@ -2858,20 +3464,28 @@
       <c r="E64">
         <v>2</v>
       </c>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="F64" t="s">
+        <v>127</v>
+      </c>
+      <c r="G64" t="s">
+        <v>126</v>
+      </c>
+      <c r="H64">
+        <v>2</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
       <c r="D65" s="1">
         <v>44913.625</v>
@@ -2879,296 +3493,309 @@
       <c r="E65">
         <v>5</v>
       </c>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
+      <c r="F65" t="s">
+        <v>110</v>
+      </c>
+      <c r="G65" t="s">
+        <v>98</v>
+      </c>
+      <c r="H65">
+        <v>3</v>
+      </c>
+      <c r="I65">
+        <v>3</v>
+      </c>
+      <c r="J65">
+        <v>4</v>
+      </c>
+      <c r="K65">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827E4A0-E10B-4512-807E-A38B484A1AB9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3177,7 +3804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619E47EA-7E3E-4F13-99F7-06A362402BF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3191,67 +3818,67 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="J2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="J3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -3259,54 +3886,54 @@
         <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="J6" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="J7" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="J8" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleared results, new results columns
</commit_message>
<xml_diff>
--- a/src/stp/database/2022-mens-world-cup.xlsx
+++ b/src/stp/database/2022-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5044102-9FF4-DF40-AA58-8CF1323F0203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2741AC2C-2F15-5C49-874F-98815F0108A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="161">
   <si>
     <t>key</t>
   </si>
@@ -509,6 +509,15 @@
   </si>
   <si>
     <t>host</t>
+  </si>
+  <si>
+    <t>home-known</t>
+  </si>
+  <si>
+    <t>away-known</t>
+  </si>
+  <si>
+    <t>after-extra-time</t>
   </si>
 </sst>
 </file>
@@ -580,10 +589,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,18 +642,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="matches" displayName="matches" ref="A1:K65" totalsRowShown="0">
-  <autoFilter ref="A1:K65" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="matches" displayName="matches" ref="A1:N65" totalsRowShown="0">
+  <autoFilter ref="A1:N65" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="match"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="time"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="venue" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="home-team"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="away-team"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="home-known">
+      <calculatedColumnFormula>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="away-known">
+      <calculatedColumnFormula>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{95F26777-3851-E845-B492-4F68AD74507C}" name="home-team"/>
+    <tableColumn id="12" xr3:uid="{7390DBEF-6468-134D-BA22-86C93C2549CC}" name="away-team"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="home-score" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="away-score" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{542D9F6A-E4A7-1B45-B170-ED109389FC8D}" name="after-extra-time"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="home-tiebreaker" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="away-tiebreaker" dataDxfId="0"/>
   </tableColumns>
@@ -1170,22 +1186,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61:K61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1202,25 +1219,34 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1237,21 +1263,15 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>QAT</v>
       </c>
       <c r="G2" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>ECU</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1268,21 +1288,15 @@
         <v>3</v>
       </c>
       <c r="F3" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>SEN</v>
       </c>
       <c r="G3" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>NED</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1299,21 +1313,15 @@
         <v>2</v>
       </c>
       <c r="F4" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ENG</v>
       </c>
       <c r="G4" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>IRN</v>
       </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1330,21 +1338,15 @@
         <v>4</v>
       </c>
       <c r="F5" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>USA</v>
       </c>
       <c r="G5" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>WAL</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1361,21 +1363,15 @@
         <v>8</v>
       </c>
       <c r="F6" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>FRA</v>
       </c>
       <c r="G6" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>AUS</v>
       </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1392,21 +1388,15 @@
         <v>7</v>
       </c>
       <c r="F7" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>DEN</v>
       </c>
       <c r="G7" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>TUN</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1423,21 +1413,15 @@
         <v>6</v>
       </c>
       <c r="F8" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>MEX</v>
       </c>
       <c r="G8" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>POL</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1454,21 +1438,15 @@
         <v>5</v>
       </c>
       <c r="F9" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ARG</v>
       </c>
       <c r="G9" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>KSA</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1485,21 +1463,15 @@
         <v>4</v>
       </c>
       <c r="F10" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>BEL</v>
       </c>
       <c r="G10" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CAN</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1516,21 +1488,15 @@
         <v>3</v>
       </c>
       <c r="F11" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ESP</v>
       </c>
       <c r="G11" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CRC</v>
       </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1547,21 +1513,15 @@
         <v>2</v>
       </c>
       <c r="F12" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>GER</v>
       </c>
       <c r="G12" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>JPN</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1578,21 +1538,15 @@
         <v>1</v>
       </c>
       <c r="F13" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>MAR</v>
       </c>
       <c r="G13" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CRO</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1609,21 +1563,15 @@
         <v>8</v>
       </c>
       <c r="F14" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>SUI</v>
       </c>
       <c r="G14" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CMR</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1640,21 +1588,15 @@
         <v>7</v>
       </c>
       <c r="F15" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>URU</v>
       </c>
       <c r="G15" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>KOR</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1671,21 +1613,15 @@
         <v>6</v>
       </c>
       <c r="F16" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>POR</v>
       </c>
       <c r="G16" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>GHA</v>
       </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1702,21 +1638,15 @@
         <v>5</v>
       </c>
       <c r="F17" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>BRA</v>
       </c>
       <c r="G17" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SRB</v>
       </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1733,21 +1663,15 @@
         <v>4</v>
       </c>
       <c r="F18" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>WAL</v>
       </c>
       <c r="G18" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>IRN</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1764,21 +1688,15 @@
         <v>3</v>
       </c>
       <c r="F19" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>QAT</v>
       </c>
       <c r="G19" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SEN</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1795,21 +1713,15 @@
         <v>2</v>
       </c>
       <c r="F20" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>NED</v>
       </c>
       <c r="G20" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>ECU</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1826,21 +1738,15 @@
         <v>1</v>
       </c>
       <c r="F21" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ENG</v>
       </c>
       <c r="G21" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>USA</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1857,21 +1763,15 @@
         <v>8</v>
       </c>
       <c r="F22" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>TUN</v>
       </c>
       <c r="G22" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>AUS</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1888,21 +1788,15 @@
         <v>7</v>
       </c>
       <c r="F23" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>POL</v>
       </c>
       <c r="G23" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>KSA</v>
       </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1919,21 +1813,15 @@
         <v>6</v>
       </c>
       <c r="F24" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>FRA</v>
       </c>
       <c r="G24" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>DEN</v>
       </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1950,21 +1838,15 @@
         <v>5</v>
       </c>
       <c r="F25" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ARG</v>
       </c>
       <c r="G25" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>MEX</v>
       </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1981,21 +1863,15 @@
         <v>4</v>
       </c>
       <c r="F26" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>JPN</v>
       </c>
       <c r="G26" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CRC</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2012,21 +1888,15 @@
         <v>3</v>
       </c>
       <c r="F27" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>BEL</v>
       </c>
       <c r="G27" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>MAR</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2043,21 +1913,15 @@
         <v>2</v>
       </c>
       <c r="F28" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CRO</v>
       </c>
       <c r="G28" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>CAN</v>
       </c>
-      <c r="H28">
-        <v>4</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2074,21 +1938,15 @@
         <v>1</v>
       </c>
       <c r="F29" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ESP</v>
       </c>
       <c r="G29" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>GER</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2105,21 +1963,15 @@
         <v>8</v>
       </c>
       <c r="F30" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CMR</v>
       </c>
       <c r="G30" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SRB</v>
       </c>
-      <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2136,21 +1988,15 @@
         <v>7</v>
       </c>
       <c r="F31" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>KOR</v>
       </c>
       <c r="G31" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>GHA</v>
       </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2167,21 +2013,15 @@
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>BRA</v>
       </c>
       <c r="G32" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SUI</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2198,21 +2038,15 @@
         <v>5</v>
       </c>
       <c r="F33" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>POR</v>
       </c>
       <c r="G33" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>URU</v>
       </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2229,21 +2063,15 @@
         <v>4</v>
       </c>
       <c r="F34" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>WAL</v>
       </c>
       <c r="G34" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>ENG</v>
       </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2260,21 +2088,15 @@
         <v>3</v>
       </c>
       <c r="F35" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>IRN</v>
       </c>
       <c r="G35" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>USA</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2291,21 +2113,15 @@
         <v>2</v>
       </c>
       <c r="F36" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>ECU</v>
       </c>
       <c r="G36" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SEN</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2322,21 +2138,15 @@
         <v>1</v>
       </c>
       <c r="F37" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>NED</v>
       </c>
       <c r="G37" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>QAT</v>
       </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2353,21 +2163,15 @@
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>AUS</v>
       </c>
       <c r="G38" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>DEN</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2384,21 +2188,15 @@
         <v>7</v>
       </c>
       <c r="F39" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>TUN</v>
       </c>
       <c r="G39" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>FRA</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2415,21 +2213,15 @@
         <v>6</v>
       </c>
       <c r="F40" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>POL</v>
       </c>
       <c r="G40" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>ARG</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2446,21 +2238,15 @@
         <v>5</v>
       </c>
       <c r="F41" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>KSA</v>
       </c>
       <c r="G41" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>MEX</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2477,21 +2263,15 @@
         <v>4</v>
       </c>
       <c r="F42" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CRO</v>
       </c>
       <c r="G42" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>BEL</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2508,21 +2288,15 @@
         <v>3</v>
       </c>
       <c r="F43" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CAN</v>
       </c>
       <c r="G43" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>MAR</v>
       </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2539,21 +2313,15 @@
         <v>2</v>
       </c>
       <c r="F44" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>JPN</v>
       </c>
       <c r="G44" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>ESP</v>
       </c>
-      <c r="H44">
-        <v>2</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2570,21 +2338,15 @@
         <v>1</v>
       </c>
       <c r="F45" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CRC</v>
       </c>
       <c r="G45" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>GER</v>
       </c>
-      <c r="H45">
-        <v>2</v>
-      </c>
-      <c r="I45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2601,21 +2363,15 @@
         <v>8</v>
       </c>
       <c r="F46" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>GHA</v>
       </c>
       <c r="G46" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>URU</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2632,21 +2388,15 @@
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>KOR</v>
       </c>
       <c r="G47" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>POR</v>
       </c>
-      <c r="H47">
-        <v>2</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2663,21 +2413,15 @@
         <v>6</v>
       </c>
       <c r="F48" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>SRB</v>
       </c>
       <c r="G48" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>SUI</v>
       </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-      <c r="I48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2694,21 +2438,15 @@
         <v>5</v>
       </c>
       <c r="F49" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
         <v>CMR</v>
       </c>
       <c r="G49" t="str">
-        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v>BRA</v>
       </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2724,20 +2462,16 @@
       <c r="E50">
         <v>2</v>
       </c>
-      <c r="F50" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" t="s">
-        <v>28</v>
-      </c>
-      <c r="H50">
-        <v>3</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F50" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G50" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2753,20 +2487,16 @@
       <c r="E51">
         <v>4</v>
       </c>
-      <c r="F51" t="s">
-        <v>44</v>
-      </c>
-      <c r="G51" t="s">
-        <v>33</v>
-      </c>
-      <c r="H51">
-        <v>2</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F51" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G51" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2782,20 +2512,16 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52">
-        <v>3</v>
-      </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F52" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G52" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2811,22 +2537,23 @@
       <c r="E53">
         <v>3</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H53" s="2">
-        <v>3</v>
-      </c>
-      <c r="I53" s="2">
-        <v>1</v>
-      </c>
+      <c r="F53" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G53" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="3"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2842,26 +2569,16 @@
       <c r="E54">
         <v>8</v>
       </c>
-      <c r="F54" t="s">
-        <v>57</v>
-      </c>
-      <c r="G54" t="s">
-        <v>61</v>
-      </c>
-      <c r="H54">
-        <v>1</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-      <c r="K54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F54" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G54" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2877,20 +2594,16 @@
       <c r="E55">
         <v>6</v>
       </c>
-      <c r="F55" t="s">
-        <v>76</v>
-      </c>
-      <c r="G55" t="s">
-        <v>69</v>
-      </c>
-      <c r="H55">
-        <v>4</v>
-      </c>
-      <c r="I55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F55" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G55" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2906,26 +2619,16 @@
       <c r="E56">
         <v>7</v>
       </c>
-      <c r="F56" t="s">
-        <v>60</v>
-      </c>
-      <c r="G56" t="s">
-        <v>52</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <v>3</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F56" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G56" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2941,20 +2644,16 @@
       <c r="E57">
         <v>5</v>
       </c>
-      <c r="F57" t="s">
-        <v>72</v>
-      </c>
-      <c r="G57" t="s">
-        <v>64</v>
-      </c>
-      <c r="H57">
-        <v>6</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F57" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G57" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2970,26 +2669,23 @@
       <c r="E58">
         <v>5</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H58" s="4">
-        <v>2</v>
-      </c>
-      <c r="I58" s="4">
-        <v>2</v>
-      </c>
-      <c r="J58" s="4">
-        <v>3</v>
-      </c>
-      <c r="K58" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F58" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G58" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="5"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3005,26 +2701,16 @@
       <c r="E59">
         <v>7</v>
       </c>
-      <c r="F59" t="s">
-        <v>61</v>
-      </c>
-      <c r="G59" t="s">
-        <v>76</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="J59">
-        <v>4</v>
-      </c>
-      <c r="K59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F59" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G59" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3040,20 +2726,16 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60" t="s">
-        <v>24</v>
-      </c>
-      <c r="G60" t="s">
-        <v>32</v>
-      </c>
-      <c r="H60">
-        <v>1</v>
-      </c>
-      <c r="I60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F60" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G60" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3069,22 +2751,23 @@
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H61" s="2">
-        <v>1</v>
-      </c>
-      <c r="I61" s="2">
-        <v>0</v>
-      </c>
+      <c r="F61" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G61" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="3"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="3"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3100,20 +2783,16 @@
       <c r="E62">
         <v>5</v>
       </c>
-      <c r="F62" t="s">
-        <v>44</v>
-      </c>
-      <c r="G62" t="s">
-        <v>61</v>
-      </c>
-      <c r="H62">
-        <v>3</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F62" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G62" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3129,20 +2808,16 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" t="s">
-        <v>60</v>
-      </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F63" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G63" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3158,20 +2833,16 @@
       <c r="E64">
         <v>2</v>
       </c>
-      <c r="F64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G64" t="s">
-        <v>60</v>
-      </c>
-      <c r="H64">
-        <v>2</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F64" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G64" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3187,23 +2858,13 @@
       <c r="E65">
         <v>5</v>
       </c>
-      <c r="F65" t="s">
-        <v>44</v>
-      </c>
-      <c r="G65" t="s">
-        <v>32</v>
-      </c>
-      <c r="H65">
-        <v>3</v>
-      </c>
-      <c r="I65">
-        <v>3</v>
-      </c>
-      <c r="J65">
-        <v>4</v>
-      </c>
-      <c r="K65">
-        <v>2</v>
+      <c r="F65" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0)),"")</f>
+        <v/>
+      </c>
+      <c r="G65" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>